<commit_message>
new data (RECOVERY Bari)
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur/Coding/projects/active/toci_sari_bari/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B2059A-5866-A64A-9E88-06AE6243E24A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A3C527-A93F-8C4D-A788-492F0E35CEB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16660" xr2:uid="{31837AF4-4A7D-B445-B66C-15B6A00E406F}"/>
+    <workbookView xWindow="2040" yWindow="-17640" windowWidth="28800" windowHeight="16580" xr2:uid="{31837AF4-4A7D-B445-B66C-15B6A00E406F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
   <si>
     <t>study</t>
   </si>
@@ -90,9 +90,6 @@
     <t>PreToVid</t>
   </si>
   <si>
-    <t>RECOVERY</t>
-  </si>
-  <si>
     <t>REMAP-CAP</t>
   </si>
   <si>
@@ -142,6 +139,18 @@
   </si>
   <si>
     <t>COV-BARRIER 2</t>
+  </si>
+  <si>
+    <t>RECOVERY Bari</t>
+  </si>
+  <si>
+    <t>Gray literature</t>
+  </si>
+  <si>
+    <t>RECOVERY Toci</t>
+  </si>
+  <si>
+    <t>RECOVERY Bari (No Toci)</t>
   </si>
 </sst>
 </file>
@@ -493,15 +502,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D274CB72-D850-C64C-ACAB-434DFBBEA9BC}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -509,7 +519,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -532,7 +542,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -555,7 +565,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -578,7 +588,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -601,7 +611,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -624,7 +634,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -647,7 +657,7 @@
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -670,7 +680,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
@@ -693,7 +703,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
@@ -716,7 +726,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -739,7 +749,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
@@ -762,7 +772,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -782,10 +792,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -805,10 +815,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -828,10 +838,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -851,10 +861,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -874,13 +884,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
         <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>23</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -897,13 +907,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D18">
         <v>27</v>
@@ -920,13 +930,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D19">
         <v>84</v>
@@ -943,13 +953,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D20">
         <v>8</v>
@@ -966,13 +976,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -989,13 +999,13 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22">
         <v>2</v>
@@ -1012,13 +1022,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -1035,13 +1045,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
         <v>29</v>
-      </c>
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" t="s">
-        <v>30</v>
       </c>
       <c r="D24">
         <v>57</v>
@@ -1058,13 +1068,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D25">
         <v>9</v>
@@ -1081,13 +1091,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26">
         <v>16</v>
@@ -1100,6 +1110,52 @@
       </c>
       <c r="G26">
         <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27">
+        <v>487</v>
+      </c>
+      <c r="E27">
+        <v>3962</v>
+      </c>
+      <c r="F27">
+        <v>523</v>
+      </c>
+      <c r="G27">
+        <v>3809</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28">
+        <v>306</v>
+      </c>
+      <c r="E28">
+        <v>2623</v>
+      </c>
+      <c r="F28">
+        <v>310</v>
+      </c>
+      <c r="G28">
+        <v>2525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update after inclusion of Lescure et al. and Karampitsakos et al. data
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur/Coding/projects/active/toci_sari_bari/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65774AB7-05F2-394D-828D-CFC94631C0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39BAB31-CE93-EC41-9B5C-799335E151BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16580" xr2:uid="{31837AF4-4A7D-B445-B66C-15B6A00E406F}"/>
+    <workbookView xWindow="2380" yWindow="-18100" windowWidth="28800" windowHeight="16560" xr2:uid="{31837AF4-4A7D-B445-B66C-15B6A00E406F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>study</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>CORIMUNO-TOCI-DEX</t>
+  </si>
+  <si>
+    <t>Lescure et al.</t>
   </si>
 </sst>
 </file>
@@ -493,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D274CB72-D850-C64C-ACAB-434DFBBEA9BC}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1084,6 +1087,26 @@
         <v>226</v>
       </c>
     </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <v>13</v>
+      </c>
+      <c r="D30">
+        <v>67</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>